<commit_message>
dev 0.0.5 change proportionality, zoom in to have a better view
</commit_message>
<xml_diff>
--- a/samples/Clolbert_NewCoding_hw_edits.xlsx
+++ b/samples/Clolbert_NewCoding_hw_edits.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/hwang/Desktop/repo/VisualDTA/samples/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5766F7E0-D9E0-F244-9F92-5F919C61DD85}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5D9B3716-BAF9-F048-B205-2B9D18703305}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="500" windowWidth="33360" windowHeight="20500" xr2:uid="{6F71E5C3-8CC6-AE45-8E9C-6448F6E85A50}"/>
   </bookViews>
@@ -38,7 +38,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1396" uniqueCount="387">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1397" uniqueCount="387">
   <si>
     <t>Thread</t>
   </si>
@@ -1757,8 +1757,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{498F1672-24D3-E243-B7EC-3A4A115E53DD}">
   <dimension ref="A1:AC106"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A73" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="AC82" sqref="AC82"/>
+    <sheetView tabSelected="1" topLeftCell="A68" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+      <selection activeCell="AC74" sqref="AC74"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="10.6640625" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -3734,8 +3734,8 @@
       <c r="J31" s="6" t="s">
         <v>367</v>
       </c>
-      <c r="K31" s="6">
-        <v>0</v>
+      <c r="K31" s="6" t="s">
+        <v>361</v>
       </c>
       <c r="L31" s="6">
         <v>2</v>

</xml_diff>